<commit_message>
Major update with slides
</commit_message>
<xml_diff>
--- a/data/schedule/schedule.xlsx
+++ b/data/schedule/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasschnetzer/Daten/Lehre/wipol_spec_BA/website_econpol/data/schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CDF2C5-9FDC-3B43-80BD-8BF4764E826B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC665612-6CDA-9A46-94B7-F0D42E3E90A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F9BD3B2F-4F88-794D-B86A-6B2451FB96A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Overview and administration</t>
   </si>
   <si>
-    <t>Introduction, data sources, and definitions</t>
-  </si>
-  <si>
     <t>Evolution of inequality</t>
   </si>
   <si>
@@ -118,6 +115,21 @@
   </si>
   <si>
     <t>atkinson2014</t>
+  </si>
+  <si>
+    <t>Slides</t>
+  </si>
+  <si>
+    <t>01_introduction</t>
+  </si>
+  <si>
+    <t>02_data</t>
+  </si>
+  <si>
+    <t>Data sources and definitions</t>
+  </si>
+  <si>
+    <t>03_evolution</t>
   </si>
 </sst>
 </file>
@@ -480,20 +492,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15577C13-38EE-F34D-AF16-EA7AE3F3C88F}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="2"/>
     <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,19 +517,22 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44848</v>
       </c>
@@ -526,11 +542,14 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44855</v>
       </c>
@@ -538,13 +557,16 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44869</v>
       </c>
@@ -552,22 +574,25 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44876</v>
       </c>
@@ -575,13 +600,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44883</v>
       </c>
@@ -589,22 +614,22 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44897</v>
       </c>
@@ -612,13 +637,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44904</v>
       </c>
@@ -626,22 +651,22 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44911</v>
       </c>
@@ -649,13 +674,13 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44918</v>
       </c>
@@ -663,22 +688,22 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10">
         <v>4</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
         <v>29</v>
       </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44939</v>
       </c>
@@ -686,13 +711,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44946</v>
       </c>
@@ -700,9 +725,9 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>